<commit_message>
Revert "added ZX correction"
This reverts commit 062ddce58d0f2c735ab2ffe3afa5e7575ffd870a.
</commit_message>
<xml_diff>
--- a/PhaseII_Configuration_template.xlsx
+++ b/PhaseII_Configuration_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\CFARS_SS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84FE0FC-5A24-42D6-9FFE-BB4A4B741062}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99E5319-325C-4475-B9A6-04717BE65387}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13308" xr2:uid="{A269487F-E818-43E3-8C7E-ED7B59939733}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>60m Wind Direction</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Triton</t>
+  </si>
+  <si>
+    <t>Zephir</t>
   </si>
   <si>
     <t>AQSystems</t>
@@ -559,7 +562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F08FE4-0760-457A-AC2E-B11E8BB556DD}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -730,7 +733,7 @@
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -743,10 +746,10 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -890,13 +893,10 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -915,27 +915,27 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -959,27 +959,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "added ZX correction""
This reverts commit a06fb5ba3fd51b544b28fdb35f0b24097d4e4fde.
</commit_message>
<xml_diff>
--- a/PhaseII_Configuration_template.xlsx
+++ b/PhaseII_Configuration_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\CFARS_SS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99E5319-325C-4475-B9A6-04717BE65387}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84FE0FC-5A24-42D6-9FFE-BB4A4B741062}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13308" xr2:uid="{A269487F-E818-43E3-8C7E-ED7B59939733}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <t>60m Wind Direction</t>
   </si>
@@ -165,9 +165,6 @@
   </si>
   <si>
     <t>Triton</t>
-  </si>
-  <si>
-    <t>Zephir</t>
   </si>
   <si>
     <t>AQSystems</t>
@@ -562,7 +559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F08FE4-0760-457A-AC2E-B11E8BB556DD}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -733,7 +730,7 @@
         <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -746,10 +743,10 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -893,10 +890,13 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -915,27 +915,27 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -959,27 +959,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>